<commit_message>
term sheet and project
</commit_message>
<xml_diff>
--- a/Pack n Pet Appendix Financials.xlsx
+++ b/Pack n Pet Appendix Financials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://twodegrees1-my.sharepoint.com/personal/rahul_kotian_slalom_com/Documents/Documents/Personal/UTD/Fall - 23/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{F3C844F2-B58D-4B37-BD6E-B056F96D0390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94D833CE-7206-4F40-A47E-0631BA1699BC}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{F3C844F2-B58D-4B37-BD6E-B056F96D0390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{531C4617-4976-4BC9-BFA1-A7D6196D8348}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{B484AC64-5681-4F67-AB9F-929646790744}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="3" xr2:uid="{B484AC64-5681-4F67-AB9F-929646790744}"/>
   </bookViews>
   <sheets>
     <sheet name="Assumptions" sheetId="11" r:id="rId1"/>
@@ -6088,7 +6088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{573F281C-B0B3-4836-B32D-B9F4989F5450}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -8067,8 +8067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB45C2BA-102A-4F7F-AFB1-662704B3A6CD}">
   <dimension ref="A1:M122"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10835,7 +10835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E220BFF-4E41-4A1B-83C1-4E1D31535396}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -11110,7 +11110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D9C0F0F-BF85-45FA-8C1B-71A5B58196D4}">
   <dimension ref="A1:M135"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -15292,7 +15292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EECCCCCE-A7F5-4CF7-BE44-78E976C0B5F7}">
   <dimension ref="A1:M88"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A71" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
@@ -17088,15 +17088,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004215DE4761E03F4AAAA21620D1616052" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3c0d613504b952c4f44aebbc54a6219b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fae77c4f-7f9b-4aff-ada3-fbcaff39b621" xmlns:ns4="48927070-ec2c-47ef-a538-d441225233ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7f11c0d316e86a3c5e922c58c7c3a3be" ns3:_="" ns4:_="">
     <xsd:import namespace="fae77c4f-7f9b-4aff-ada3-fbcaff39b621"/>
@@ -17319,6 +17310,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A91E8C8B-7276-4FF8-A05B-CDE38FB36D00}">
   <ds:schemaRefs>
@@ -17337,14 +17337,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB2B9B0-E6E5-4B72-933C-20D64028A100}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EDEFDFC-5B08-4CAF-851C-1DD2CDB744D9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17361,4 +17353,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB2B9B0-E6E5-4B72-933C-20D64028A100}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>